<commit_message>
Km calculation NM2-2 Day1
</commit_message>
<xml_diff>
--- a/pp_gas_enrichments/NM2_2_KmCalc_5gDry.xlsb.xlsx
+++ b/pp_gas_enrichments/NM2_2_KmCalc_5gDry.xlsb.xlsx
@@ -20,6 +20,74 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ethylene injections yesterday affected the methanizer, methane readings seem to be unaffected</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Due to ethylene injections yesterday CO2 sensitivity has dropped at about 50%</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
   <si>
@@ -60,7 +128,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +157,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -114,12 +195,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -402,11 +483,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AD10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="O4:P4"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,44 +496,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:30" x14ac:dyDescent="0.25">
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3" t="s">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3" t="s">
+      <c r="N2" s="6"/>
+      <c r="O2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
     </row>
     <row r="3" spans="3:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -498,70 +579,108 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="5">
+    <row r="4" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="4">
         <v>42968</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>2767</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>7076.52</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>2675</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>6841</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>30.63</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>78.37</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>34.36</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>87.9</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <v>5.89</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>15.096</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <v>5.12</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="3">
         <v>13.13</v>
       </c>
     </row>
-    <row r="5" spans="3:30" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="3:30" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="3:30" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="3:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="3:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
+    <row r="5" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="4">
+        <v>42969</v>
+      </c>
+      <c r="D5" s="3">
+        <f>C5-C4</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2734</v>
+      </c>
+      <c r="F5" s="3">
+        <v>7077.67</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2633.64</v>
+      </c>
+      <c r="H5" s="3">
+        <v>6816.12</v>
+      </c>
+      <c r="I5" s="3">
+        <v>25.01</v>
+      </c>
+      <c r="J5" s="3">
+        <v>64.489999999999995</v>
+      </c>
+      <c r="K5" s="3">
+        <v>24.01</v>
+      </c>
+      <c r="L5" s="3">
+        <v>61.9</v>
+      </c>
+      <c r="M5" s="3">
+        <v>3</v>
+      </c>
+      <c r="N5" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="O5" s="3">
+        <v>3.42</v>
+      </c>
+      <c r="P5" s="3">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="6" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="3:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="6"/>
+      <c r="C10" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
@@ -569,18 +688,25 @@
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:P2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,20 +743,20 @@
         <v>10</v>
       </c>
       <c r="P2" s="7"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
     </row>
     <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -676,63 +802,112 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="5">
+    <row r="4" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="4">
         <v>42968</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>29.7</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0.05</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>46.2</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>8.4199999999999997E-2</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>27.59</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>5.0299999999999997E-2</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>37.25</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>6.7900000000000002E-2</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <v>23.8</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>4.3400000000000001E-2</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <v>23.9</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="3">
         <v>4.3700000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="5"/>
+    <row r="5" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="4">
+        <v>42969</v>
+      </c>
+      <c r="D5" s="3">
+        <f>C5-C4</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>22.8</v>
+      </c>
+      <c r="F5" s="3">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>21.05</v>
+      </c>
+      <c r="H5" s="3">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="I5" s="3">
+        <v>21.47</v>
+      </c>
+      <c r="J5" s="3">
+        <v>7.4300000000000005E-2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>20.05</v>
+      </c>
+      <c r="L5" s="3">
+        <v>6.9400000000000003E-2</v>
+      </c>
+      <c r="M5" s="3">
+        <v>19.86</v>
+      </c>
+      <c r="N5" s="3">
+        <v>6.88E-2</v>
+      </c>
+      <c r="O5" s="3">
+        <v>19.739999999999998</v>
+      </c>
+      <c r="P5" s="3">
+        <v>6.83E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="AC2:AD2"/>
@@ -741,13 +916,9 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more of ch4/ethylene data
</commit_message>
<xml_diff>
--- a/pp_gas_enrichments/NM2_2_KmCalc_5gDry.xlsb.xlsx
+++ b/pp_gas_enrichments/NM2_2_KmCalc_5gDry.xlsb.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH4" sheetId="2" r:id="rId1"/>
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -34,7 +34,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -43,10 +43,227 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 ethylene injections yesterday affected the methanizer, methane readings seem to be unaffected</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+overestimates, perhaps GC wasn't accurate in the  beginning</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Values were lower, but after re-running a couple times it equilibrated there</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+refilled #5, 6 with 1 ml of pure ch4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{32475D15-5BB2-4407-A031-E9129B5E9BB6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+It seem that ch4 sensitivity declined, for high concentrations and CO2 sensetivity increased</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N10" authorId="0" shapeId="0" xr:uid="{86655BB5-8DC9-4816-9A01-5518F72DD4C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+it was 816. according to the new calibration that underestimated. Used old(day5) calibration to obtain 796.9</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P10" authorId="0" shapeId="0" xr:uid="{5C325821-BF21-4BEE-B02E-7288C26EAB4E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+it was 786.38 according to the new calibration that underestimated. Used old(day5) calibration to obtain 765</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{51C5B48C-0742-4862-A5DE-0C198BA79505}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Calibrations seem to be magically back to normal, probably the air compressor thing</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{4D40D526-D629-401B-8531-55A401152433}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ch4 0.5% standard starts low but then after ~1 h goes back to 1920</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{EC6A3FB4-21B1-4471-83CE-5CDBC9417C1C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+recalibrated GC
+</t>
         </r>
       </text>
     </comment>
@@ -55,12 +272,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -68,7 +285,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -77,10 +294,58 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Due to ethylene injections yesterday CO2 sensitivity has dropped at about 50%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+refilled #5, 6 with 1 ml of pure ch4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{099A824F-C5D5-455D-A0B3-AF0B9539804E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+calibration seems to be back at 1920-30 per 0.5% ch4, I guess compressor has cleaned from methane contaminated air</t>
         </r>
       </text>
     </comment>
@@ -127,8 +392,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,14 +410,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,13 +469,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,11 +763,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:AD10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C2:AD16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,44 +776,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:30" x14ac:dyDescent="0.25">
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6" t="s">
+      <c r="L2" s="8"/>
+      <c r="M2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6" t="s">
+      <c r="N2" s="8"/>
+      <c r="O2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
     </row>
     <row r="3" spans="3:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -579,108 +859,497 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="4">
+    <row r="4" spans="3:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
         <v>42968</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>2767</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>7076.52</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>2675</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>6841</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>30.63</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>78.37</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>34.36</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>87.9</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <v>5.89</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>15.096</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="2">
         <v>5.12</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="2">
         <v>13.13</v>
       </c>
     </row>
-    <row r="5" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="4">
+    <row r="5" spans="3:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
         <v>42969</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <f>C5-C4</f>
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>2734</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>7077.67</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>2633.64</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>6816.12</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>25.01</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>64.489999999999995</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>24.01</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>61.9</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <v>3</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>7.6</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="2">
         <v>3.42</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="2">
         <v>8.6</v>
       </c>
     </row>
-    <row r="6" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="3:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="4"/>
+    <row r="6" spans="3:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <v>42970</v>
+      </c>
+      <c r="D6" s="2">
+        <f>C6-C4</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2689</v>
+      </c>
+      <c r="F6" s="4">
+        <v>6993.69</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2612.81</v>
+      </c>
+      <c r="H6" s="4">
+        <v>6795.26</v>
+      </c>
+      <c r="I6" s="2">
+        <v>23.02</v>
+      </c>
+      <c r="J6" s="2">
+        <v>59.5</v>
+      </c>
+      <c r="K6" s="2">
+        <v>21.92</v>
+      </c>
+      <c r="L6" s="2">
+        <v>56.6</v>
+      </c>
+      <c r="M6" s="2">
+        <v>2.1480000000000001</v>
+      </c>
+      <c r="N6" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="O6" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="P6" s="2">
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="7" spans="3:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>42972</v>
+      </c>
+      <c r="D7" s="2">
+        <f>C7-C4</f>
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2705</v>
+      </c>
+      <c r="F7" s="2">
+        <v>7033.53</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2627</v>
+      </c>
+      <c r="H7" s="2">
+        <v>6831.46</v>
+      </c>
+      <c r="I7" s="2">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="J7" s="2">
+        <v>45.19</v>
+      </c>
+      <c r="K7" s="2">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="L7" s="2">
+        <v>43.91</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1.097</v>
+      </c>
+      <c r="N7" s="2">
+        <v>2.7926000000000002</v>
+      </c>
+      <c r="O7" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="P7" s="2">
+        <v>4.3899999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="3:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>42973</v>
+      </c>
+      <c r="D8" s="2">
+        <f>C8-C4</f>
+        <v>5</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="N8" s="2">
+        <v>2.38</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="P8" s="2">
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="3:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <v>42973</v>
+      </c>
+      <c r="D9" s="2">
+        <f>C9-C4</f>
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2748.77</v>
+      </c>
+      <c r="F9" s="2">
+        <v>7089.36</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2657.39</v>
+      </c>
+      <c r="H9" s="2">
+        <v>6853.67</v>
+      </c>
+      <c r="I9" s="2">
+        <v>16.12</v>
+      </c>
+      <c r="J9" s="2">
+        <v>41.29</v>
+      </c>
+      <c r="K9" s="2">
+        <v>15.15</v>
+      </c>
+      <c r="L9" s="2">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="M9" s="2">
+        <v>311.5</v>
+      </c>
+      <c r="N9" s="2">
+        <v>803.13</v>
+      </c>
+      <c r="O9" s="2">
+        <v>300.3</v>
+      </c>
+      <c r="P9" s="2">
+        <v>774.26</v>
+      </c>
     </row>
     <row r="10" spans="3:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
+      <c r="C10" s="3">
+        <v>42975</v>
+      </c>
+      <c r="D10" s="2">
+        <f>C10-C4</f>
+        <v>7</v>
+      </c>
+      <c r="I10" s="2">
+        <v>11.95</v>
+      </c>
+      <c r="J10" s="2">
+        <v>31.31</v>
+      </c>
+      <c r="K10" s="2">
+        <v>10.46</v>
+      </c>
+      <c r="L10" s="2">
+        <v>27.36</v>
+      </c>
+      <c r="M10" s="2">
+        <v>309.11</v>
+      </c>
+      <c r="N10" s="6">
+        <f>M10*N9/M9</f>
+        <v>796.96794317817023</v>
+      </c>
+      <c r="O10" s="2">
+        <v>296.99</v>
+      </c>
+      <c r="P10" s="6">
+        <f>O10*P9/O9</f>
+        <v>765.72586546786545</v>
+      </c>
+    </row>
+    <row r="11" spans="3:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="7">
+        <v>42975</v>
+      </c>
+      <c r="D11" s="6">
+        <f>C11-C4</f>
+        <v>7</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2677</v>
+      </c>
+      <c r="F11" s="6">
+        <v>6932.7</v>
+      </c>
+      <c r="G11" s="6">
+        <v>2614</v>
+      </c>
+      <c r="H11" s="6">
+        <v>6770</v>
+      </c>
+      <c r="M11" s="6">
+        <v>307.26</v>
+      </c>
+      <c r="N11" s="6">
+        <v>795.36</v>
+      </c>
+      <c r="O11" s="6">
+        <v>296.92</v>
+      </c>
+      <c r="P11" s="6">
+        <v>768.57</v>
+      </c>
+    </row>
+    <row r="12" spans="3:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="7">
+        <v>42977</v>
+      </c>
+      <c r="D12" s="6">
+        <f>C12-C4</f>
+        <v>9</v>
+      </c>
+      <c r="E12" s="6">
+        <v>2602</v>
+      </c>
+      <c r="F12" s="6">
+        <v>6771</v>
+      </c>
+      <c r="G12" s="6">
+        <v>2578.6999999999998</v>
+      </c>
+      <c r="H12" s="6">
+        <v>6709.28</v>
+      </c>
+      <c r="I12" s="2">
+        <v>9.19</v>
+      </c>
+      <c r="J12" s="2">
+        <v>22.46</v>
+      </c>
+      <c r="K12" s="6">
+        <v>6.29</v>
+      </c>
+      <c r="L12" s="6">
+        <v>14.73</v>
+      </c>
+      <c r="M12" s="6">
+        <v>291.8</v>
+      </c>
+      <c r="N12" s="6">
+        <v>757.95</v>
+      </c>
+      <c r="O12" s="6">
+        <v>282.7389</v>
+      </c>
+      <c r="P12" s="6">
+        <v>734.37</v>
+      </c>
+    </row>
+    <row r="13" spans="3:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="7">
+        <v>42978</v>
+      </c>
+      <c r="D13" s="6">
+        <f>C13-C4</f>
+        <v>10</v>
+      </c>
+      <c r="I13" s="6">
+        <v>5.87</v>
+      </c>
+      <c r="J13" s="6">
+        <v>14.47</v>
+      </c>
+      <c r="K13" s="6">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="L13" s="6">
+        <v>11.77</v>
+      </c>
+      <c r="M13" s="6">
+        <v>291.54000000000002</v>
+      </c>
+      <c r="N13" s="6">
+        <v>762.54</v>
+      </c>
+      <c r="O13" s="6">
+        <v>282.31</v>
+      </c>
+      <c r="P13" s="6">
+        <v>738.37</v>
+      </c>
+    </row>
+    <row r="14" spans="3:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="7">
+        <v>42978</v>
+      </c>
+      <c r="D14" s="6">
+        <f>C14-C4</f>
+        <v>10</v>
+      </c>
+      <c r="E14" s="6">
+        <v>2618.83</v>
+      </c>
+      <c r="F14" s="6">
+        <v>6872.34</v>
+      </c>
+      <c r="G14" s="6">
+        <v>2561.06</v>
+      </c>
+      <c r="H14" s="6">
+        <v>6720.74</v>
+      </c>
+      <c r="M14" s="6">
+        <v>290.25</v>
+      </c>
+      <c r="N14" s="6">
+        <v>760.8</v>
+      </c>
+      <c r="O14" s="6">
+        <v>283</v>
+      </c>
+      <c r="P14" s="6">
+        <v>742.13</v>
+      </c>
+    </row>
+    <row r="15" spans="3:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="7">
+        <v>42979</v>
+      </c>
+      <c r="D15" s="6">
+        <f>C15-C4</f>
+        <v>11</v>
+      </c>
+      <c r="E15" s="6">
+        <v>2675</v>
+      </c>
+      <c r="F15" s="6">
+        <v>7030.02</v>
+      </c>
+      <c r="I15" s="6">
+        <v>5.25</v>
+      </c>
+      <c r="J15" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="K15" s="6">
+        <v>3.387</v>
+      </c>
+      <c r="L15" s="6">
+        <v>7.5869</v>
+      </c>
+      <c r="M15" s="6">
+        <v>290.23</v>
+      </c>
+      <c r="N15" s="6">
+        <v>761.56</v>
+      </c>
+      <c r="O15" s="6">
+        <v>280.20999999999998</v>
+      </c>
+      <c r="P15" s="6">
+        <v>735.21</v>
+      </c>
+    </row>
+    <row r="16" spans="3:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="5">
+        <v>42979</v>
+      </c>
+      <c r="D16" s="1">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2677</v>
+      </c>
+      <c r="F16" s="1">
+        <v>7036</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2575</v>
+      </c>
+      <c r="H16" s="1">
+        <v>6768.14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
@@ -688,12 +1357,6 @@
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:P2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -702,11 +1365,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AD9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:AD14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,44 +1382,44 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7" t="s">
+      <c r="L2" s="9"/>
+      <c r="M2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7" t="s">
+      <c r="N2" s="9"/>
+      <c r="O2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
     </row>
     <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -802,112 +1465,426 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="4">
+    <row r="4" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
         <v>42968</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>29.7</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0.05</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>46.2</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>8.4199999999999997E-2</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>27.59</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>5.0299999999999997E-2</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>37.25</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>6.7900000000000002E-2</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <v>23.8</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>4.3400000000000001E-2</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="2">
         <v>23.9</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="2">
         <v>4.3700000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="4">
+    <row r="5" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
         <v>42969</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <f>C5-C4</f>
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>22.8</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>21.05</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>7.2900000000000006E-2</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>21.47</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>7.4300000000000005E-2</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>20.05</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>6.9400000000000003E-2</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <v>19.86</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>6.88E-2</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="2">
         <v>19.739999999999998</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="2">
         <v>6.83E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="4"/>
+    <row r="6" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <v>42970</v>
+      </c>
+      <c r="D6" s="2">
+        <f>C6-C4</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>24.57</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8.4400000000000003E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>23.46</v>
+      </c>
+      <c r="H6" s="2">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>21.96</v>
+      </c>
+      <c r="J6" s="2">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>25.28</v>
+      </c>
+      <c r="L6" s="2">
+        <v>8.6900000000000005E-2</v>
+      </c>
+      <c r="M6" s="2">
+        <v>21.64</v>
+      </c>
+      <c r="N6" s="2">
+        <v>7.4399999999999994E-2</v>
+      </c>
+      <c r="O6" s="2">
+        <v>22.3</v>
+      </c>
+      <c r="P6" s="2">
+        <v>7.6700000000000004E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>42972</v>
+      </c>
+      <c r="D7" s="2">
+        <f>C7-C4</f>
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>24.92</v>
+      </c>
+      <c r="F7" s="2">
+        <v>9.5399999999999999E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>24.24</v>
+      </c>
+      <c r="H7" s="2">
+        <v>9.2799999999999994E-2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>22.93</v>
+      </c>
+      <c r="J7" s="2">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>22.005400000000002</v>
+      </c>
+      <c r="L7" s="2">
+        <v>8.4199999999999997E-2</v>
+      </c>
+      <c r="M7" s="2">
+        <v>22.1</v>
+      </c>
+      <c r="N7" s="2">
+        <v>8.4599999999999995E-2</v>
+      </c>
+      <c r="O7" s="2">
+        <v>25.84</v>
+      </c>
+      <c r="P7" s="2">
+        <v>9.8900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>42973</v>
+      </c>
+      <c r="D8" s="2">
+        <f>C8-C4</f>
+        <v>5</v>
+      </c>
+      <c r="M8" s="2">
+        <v>28.35</v>
+      </c>
+      <c r="N8" s="2">
+        <v>9.4299999999999995E-2</v>
+      </c>
+      <c r="O8" s="2">
+        <v>29.04</v>
+      </c>
+      <c r="P8" s="2">
+        <v>9.6600000000000005E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
+      <c r="C9" s="3">
+        <v>42973</v>
+      </c>
+      <c r="D9" s="2">
+        <f>C9-C4</f>
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>27.01</v>
+      </c>
+      <c r="F9" s="2">
+        <v>9.3700000000000006E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>26.77</v>
+      </c>
+      <c r="H9" s="2">
+        <v>9.2799999999999994E-2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>27.31</v>
+      </c>
+      <c r="J9" s="2">
+        <v>9.4700000000000006E-2</v>
+      </c>
+      <c r="K9" s="2">
+        <v>28.4</v>
+      </c>
+      <c r="L9" s="2">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="M9" s="2">
+        <v>27.01</v>
+      </c>
+      <c r="N9" s="2">
+        <v>9.3700000000000006E-2</v>
+      </c>
+      <c r="O9" s="2">
+        <v>28.39</v>
+      </c>
+      <c r="P9" s="2">
+        <v>9.8400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="7">
+        <v>42975</v>
+      </c>
+      <c r="D10" s="6">
+        <f>C10-C4</f>
+        <v>7</v>
+      </c>
+      <c r="E10" s="6">
+        <v>38.08</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="I10" s="6">
+        <v>37.4</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.1149</v>
+      </c>
+      <c r="K10" s="6">
+        <v>35.479999999999997</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0.109</v>
+      </c>
+      <c r="M10" s="6">
+        <v>36.04</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="O10" s="6">
+        <v>43.01</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0.1321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="7">
+        <v>42975</v>
+      </c>
+      <c r="G11" s="6">
+        <v>31.45</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.1145</v>
+      </c>
+      <c r="M11" s="6">
+        <v>30.88</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0.1124</v>
+      </c>
+      <c r="O11" s="6">
+        <v>32</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0.1168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="7">
+        <v>42977</v>
+      </c>
+      <c r="D12" s="6">
+        <f>C12-C4</f>
+        <v>9</v>
+      </c>
+      <c r="E12" s="6">
+        <v>44.2</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.12230000000000001</v>
+      </c>
+      <c r="G12" s="6">
+        <v>41.62</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.115</v>
+      </c>
+      <c r="I12" s="6">
+        <v>45.02</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.12529999999999999</v>
+      </c>
+      <c r="K12" s="6">
+        <v>47.08</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="M12" s="6">
+        <v>42.94</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0.1188</v>
+      </c>
+      <c r="O12" s="6">
+        <v>43.59</v>
+      </c>
+      <c r="P12" s="6">
+        <v>0.1206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="7">
+        <v>42978</v>
+      </c>
+      <c r="D13" s="6">
+        <f>C13-C4</f>
+        <v>10</v>
+      </c>
+      <c r="I13" s="6">
+        <v>41.56</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0.12239999999999999</v>
+      </c>
+      <c r="K13" s="6">
+        <v>39.729999999999997</v>
+      </c>
+      <c r="L13" s="6">
+        <v>0.11700000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="5">
+        <v>42979</v>
+      </c>
+      <c r="D14" s="1">
+        <f>C14-C4</f>
+        <v>11</v>
+      </c>
+      <c r="E14" s="1">
+        <v>50.77</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.14940000000000001</v>
+      </c>
+      <c r="G14" s="1">
+        <v>44.75</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.1293</v>
+      </c>
+      <c r="I14" s="1">
+        <v>47.036999999999999</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.13589999999999999</v>
+      </c>
+      <c r="K14" s="1">
+        <v>44.3</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.128</v>
+      </c>
+      <c r="M14" s="1">
+        <v>44.56</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0.12870000000000001</v>
+      </c>
+      <c r="O14" s="1">
+        <v>49.39</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0.1452</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="AC2:AD2"/>
@@ -916,6 +1893,11 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Km and ethylene cont.
</commit_message>
<xml_diff>
--- a/pp_gas_enrichments/NM2_2_KmCalc_5gDry.xlsb.xlsx
+++ b/pp_gas_enrichments/NM2_2_KmCalc_5gDry.xlsb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH4" sheetId="2" r:id="rId1"/>
@@ -264,6 +264,30 @@
           <t xml:space="preserve">
 recalibrated GC
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{970FB299-65CC-4A3E-8946-61A5DF400B4A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+calibration seems to be good, 1930 for o.5% ch4</t>
         </r>
       </text>
     </comment>
@@ -764,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:AD16"/>
+  <dimension ref="C2:AD17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,34 +1346,73 @@
         <v>735.21</v>
       </c>
     </row>
-    <row r="16" spans="3:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="5">
+    <row r="16" spans="3:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="7">
         <v>42979</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="6">
         <v>11</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="6">
         <v>2677</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="6">
         <v>7036</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="6">
         <v>2575</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="6">
         <v>6768.14</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="5">
+        <v>42982</v>
+      </c>
+      <c r="D17" s="1">
+        <f>C17-C4</f>
+        <v>14</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2718.17</v>
+      </c>
+      <c r="F17" s="1">
+        <v>7038.63</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2628</v>
+      </c>
+      <c r="H17" s="1">
+        <v>6807.5</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1.98</v>
+      </c>
+      <c r="J17" s="1">
+        <v>4.07</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1.21</v>
+      </c>
+      <c r="L17" s="1">
+        <v>2.0594999999999999</v>
+      </c>
+      <c r="M17" s="1">
+        <v>284.19</v>
+      </c>
+      <c r="N17" s="1">
+        <v>734.93</v>
+      </c>
+      <c r="O17" s="1">
+        <v>278.5</v>
+      </c>
+      <c r="P17" s="1">
+        <v>720.32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
@@ -1357,6 +1420,12 @@
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:P2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1366,10 +1435,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:AD14"/>
+  <dimension ref="A2:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,53 +1907,103 @@
         <v>0.11700000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="5">
+    <row r="14" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="7">
         <v>42979</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="6">
         <f>C14-C4</f>
         <v>11</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="6">
         <v>50.77</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="6">
         <v>0.14940000000000001</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="6">
         <v>44.75</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="6">
         <v>0.1293</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="6">
         <v>47.036999999999999</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="6">
         <v>0.13589999999999999</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="6">
         <v>44.3</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="6">
         <v>0.128</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="6">
         <v>44.56</v>
       </c>
-      <c r="N14" s="1">
+      <c r="N14" s="6">
         <v>0.12870000000000001</v>
       </c>
-      <c r="O14" s="1">
+      <c r="O14" s="6">
         <v>49.39</v>
       </c>
-      <c r="P14" s="1">
+      <c r="P14" s="6">
         <v>0.1452</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="5">
+        <v>42982</v>
+      </c>
+      <c r="D15" s="1">
+        <f>C15-C4</f>
+        <v>14</v>
+      </c>
+      <c r="E15" s="1">
+        <v>79.88</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.15040000000000001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>74.5</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.14030000000000001</v>
+      </c>
+      <c r="I15" s="1">
+        <v>78.150000000000006</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="K15" s="1">
+        <v>71.19</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="M15" s="1">
+        <v>67.540000000000006</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0.12720000000000001</v>
+      </c>
+      <c r="O15" s="1">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0.15240000000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="AC2:AD2"/>
@@ -1893,11 +2012,6 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>